<commit_message>
README, BOM, image updates
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BGM111 Programmer" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>SiLabs BGM111 External Programmer BOM</t>
+  </si>
   <si>
     <t>Designator:</t>
   </si>
@@ -80,7 +83,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.0000;[RED]\-[$$-409]#,##0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -106,6 +109,13 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -178,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,35 +201,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -240,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -259,28 +273,16 @@
     <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
@@ -1294,55 +1296,1062 @@
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+      <c r="AY2" s="0"/>
+      <c r="AZ2" s="0"/>
+      <c r="BA2" s="0"/>
+      <c r="BB2" s="0"/>
+      <c r="BC2" s="0"/>
+      <c r="BD2" s="0"/>
+      <c r="BE2" s="0"/>
+      <c r="BF2" s="0"/>
+      <c r="BG2" s="0"/>
+      <c r="BH2" s="0"/>
+      <c r="BI2" s="0"/>
+      <c r="BJ2" s="0"/>
+      <c r="BK2" s="0"/>
+      <c r="BL2" s="0"/>
+      <c r="BM2" s="0"/>
+      <c r="BN2" s="0"/>
+      <c r="BO2" s="0"/>
+      <c r="BP2" s="0"/>
+      <c r="BQ2" s="0"/>
+      <c r="BR2" s="0"/>
+      <c r="BS2" s="0"/>
+      <c r="BT2" s="0"/>
+      <c r="BU2" s="0"/>
+      <c r="BV2" s="0"/>
+      <c r="BW2" s="0"/>
+      <c r="BX2" s="0"/>
+      <c r="BY2" s="0"/>
+      <c r="BZ2" s="0"/>
+      <c r="CA2" s="0"/>
+      <c r="CB2" s="0"/>
+      <c r="CC2" s="0"/>
+      <c r="CD2" s="0"/>
+      <c r="CE2" s="0"/>
+      <c r="CF2" s="0"/>
+      <c r="CG2" s="0"/>
+      <c r="CH2" s="0"/>
+      <c r="CI2" s="0"/>
+      <c r="CJ2" s="0"/>
+      <c r="CK2" s="0"/>
+      <c r="CL2" s="0"/>
+      <c r="CM2" s="0"/>
+      <c r="CN2" s="0"/>
+      <c r="CO2" s="0"/>
+      <c r="CP2" s="0"/>
+      <c r="CQ2" s="0"/>
+      <c r="CR2" s="0"/>
+      <c r="CS2" s="0"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="0"/>
+      <c r="CV2" s="0"/>
+      <c r="CW2" s="0"/>
+      <c r="CX2" s="0"/>
+      <c r="CY2" s="0"/>
+      <c r="CZ2" s="0"/>
+      <c r="DA2" s="0"/>
+      <c r="DB2" s="0"/>
+      <c r="DC2" s="0"/>
+      <c r="DD2" s="0"/>
+      <c r="DE2" s="0"/>
+      <c r="DF2" s="0"/>
+      <c r="DG2" s="0"/>
+      <c r="DH2" s="0"/>
+      <c r="DI2" s="0"/>
+      <c r="DJ2" s="0"/>
+      <c r="DK2" s="0"/>
+      <c r="DL2" s="0"/>
+      <c r="DM2" s="0"/>
+      <c r="DN2" s="0"/>
+      <c r="DO2" s="0"/>
+      <c r="DP2" s="0"/>
+      <c r="DQ2" s="0"/>
+      <c r="DR2" s="0"/>
+      <c r="DS2" s="0"/>
+      <c r="DT2" s="0"/>
+      <c r="DU2" s="0"/>
+      <c r="DV2" s="0"/>
+      <c r="DW2" s="0"/>
+      <c r="DX2" s="0"/>
+      <c r="DY2" s="0"/>
+      <c r="DZ2" s="0"/>
+      <c r="EA2" s="0"/>
+      <c r="EB2" s="0"/>
+      <c r="EC2" s="0"/>
+      <c r="ED2" s="0"/>
+      <c r="EE2" s="0"/>
+      <c r="EF2" s="0"/>
+      <c r="EG2" s="0"/>
+      <c r="EH2" s="0"/>
+      <c r="EI2" s="0"/>
+      <c r="EJ2" s="0"/>
+      <c r="EK2" s="0"/>
+      <c r="EL2" s="0"/>
+      <c r="EM2" s="0"/>
+      <c r="EN2" s="0"/>
+      <c r="EO2" s="0"/>
+      <c r="EP2" s="0"/>
+      <c r="EQ2" s="0"/>
+      <c r="ER2" s="0"/>
+      <c r="ES2" s="0"/>
+      <c r="ET2" s="0"/>
+      <c r="EU2" s="0"/>
+      <c r="EV2" s="0"/>
+      <c r="EW2" s="0"/>
+      <c r="EX2" s="0"/>
+      <c r="EY2" s="0"/>
+      <c r="EZ2" s="0"/>
+      <c r="FA2" s="0"/>
+      <c r="FB2" s="0"/>
+      <c r="FC2" s="0"/>
+      <c r="FD2" s="0"/>
+      <c r="FE2" s="0"/>
+      <c r="FF2" s="0"/>
+      <c r="FG2" s="0"/>
+      <c r="FH2" s="0"/>
+      <c r="FI2" s="0"/>
+      <c r="FJ2" s="0"/>
+      <c r="FK2" s="0"/>
+      <c r="FL2" s="0"/>
+      <c r="FM2" s="0"/>
+      <c r="FN2" s="0"/>
+      <c r="FO2" s="0"/>
+      <c r="FP2" s="0"/>
+      <c r="FQ2" s="0"/>
+      <c r="FR2" s="0"/>
+      <c r="FS2" s="0"/>
+      <c r="FT2" s="0"/>
+      <c r="FU2" s="0"/>
+      <c r="FV2" s="0"/>
+      <c r="FW2" s="0"/>
+      <c r="FX2" s="0"/>
+      <c r="FY2" s="0"/>
+      <c r="FZ2" s="0"/>
+      <c r="GA2" s="0"/>
+      <c r="GB2" s="0"/>
+      <c r="GC2" s="0"/>
+      <c r="GD2" s="0"/>
+      <c r="GE2" s="0"/>
+      <c r="GF2" s="0"/>
+      <c r="GG2" s="0"/>
+      <c r="GH2" s="0"/>
+      <c r="GI2" s="0"/>
+      <c r="GJ2" s="0"/>
+      <c r="GK2" s="0"/>
+      <c r="GL2" s="0"/>
+      <c r="GM2" s="0"/>
+      <c r="GN2" s="0"/>
+      <c r="GO2" s="0"/>
+      <c r="GP2" s="0"/>
+      <c r="GQ2" s="0"/>
+      <c r="GR2" s="0"/>
+      <c r="GS2" s="0"/>
+      <c r="GT2" s="0"/>
+      <c r="GU2" s="0"/>
+      <c r="GV2" s="0"/>
+      <c r="GW2" s="0"/>
+      <c r="GX2" s="0"/>
+      <c r="GY2" s="0"/>
+      <c r="GZ2" s="0"/>
+      <c r="HA2" s="0"/>
+      <c r="HB2" s="0"/>
+      <c r="HC2" s="0"/>
+      <c r="HD2" s="0"/>
+      <c r="HE2" s="0"/>
+      <c r="HF2" s="0"/>
+      <c r="HG2" s="0"/>
+      <c r="HH2" s="0"/>
+      <c r="HI2" s="0"/>
+      <c r="HJ2" s="0"/>
+      <c r="HK2" s="0"/>
+      <c r="HL2" s="0"/>
+      <c r="HM2" s="0"/>
+      <c r="HN2" s="0"/>
+      <c r="HO2" s="0"/>
+      <c r="HP2" s="0"/>
+      <c r="HQ2" s="0"/>
+      <c r="HR2" s="0"/>
+      <c r="HS2" s="0"/>
+      <c r="HT2" s="0"/>
+      <c r="HU2" s="0"/>
+      <c r="HV2" s="0"/>
+      <c r="HW2" s="0"/>
+      <c r="HX2" s="0"/>
+      <c r="HY2" s="0"/>
+      <c r="HZ2" s="0"/>
+      <c r="IA2" s="0"/>
+      <c r="IB2" s="0"/>
+      <c r="IC2" s="0"/>
+      <c r="ID2" s="0"/>
+      <c r="IE2" s="0"/>
+      <c r="IF2" s="0"/>
+      <c r="IG2" s="0"/>
+      <c r="IH2" s="0"/>
+      <c r="II2" s="0"/>
+      <c r="IJ2" s="0"/>
+      <c r="IK2" s="0"/>
+      <c r="IL2" s="0"/>
+      <c r="IM2" s="0"/>
+      <c r="IN2" s="0"/>
+      <c r="IO2" s="0"/>
+      <c r="IP2" s="0"/>
+      <c r="IQ2" s="0"/>
+      <c r="IR2" s="0"/>
+      <c r="IS2" s="0"/>
+      <c r="IT2" s="0"/>
+      <c r="IU2" s="0"/>
+      <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
+      <c r="IX2" s="0"/>
+      <c r="IY2" s="0"/>
+      <c r="IZ2" s="0"/>
+      <c r="JA2" s="0"/>
+      <c r="JB2" s="0"/>
+      <c r="JC2" s="0"/>
+      <c r="JD2" s="0"/>
+      <c r="JE2" s="0"/>
+      <c r="JF2" s="0"/>
+      <c r="JG2" s="0"/>
+      <c r="JH2" s="0"/>
+      <c r="JI2" s="0"/>
+      <c r="JJ2" s="0"/>
+      <c r="JK2" s="0"/>
+      <c r="JL2" s="0"/>
+      <c r="JM2" s="0"/>
+      <c r="JN2" s="0"/>
+      <c r="JO2" s="0"/>
+      <c r="JP2" s="0"/>
+      <c r="JQ2" s="0"/>
+      <c r="JR2" s="0"/>
+      <c r="JS2" s="0"/>
+      <c r="JT2" s="0"/>
+      <c r="JU2" s="0"/>
+      <c r="JV2" s="0"/>
+      <c r="JW2" s="0"/>
+      <c r="JX2" s="0"/>
+      <c r="JY2" s="0"/>
+      <c r="JZ2" s="0"/>
+      <c r="KA2" s="0"/>
+      <c r="KB2" s="0"/>
+      <c r="KC2" s="0"/>
+      <c r="KD2" s="0"/>
+      <c r="KE2" s="0"/>
+      <c r="KF2" s="0"/>
+      <c r="KG2" s="0"/>
+      <c r="KH2" s="0"/>
+      <c r="KI2" s="0"/>
+      <c r="KJ2" s="0"/>
+      <c r="KK2" s="0"/>
+      <c r="KL2" s="0"/>
+      <c r="KM2" s="0"/>
+      <c r="KN2" s="0"/>
+      <c r="KO2" s="0"/>
+      <c r="KP2" s="0"/>
+      <c r="KQ2" s="0"/>
+      <c r="KR2" s="0"/>
+      <c r="KS2" s="0"/>
+      <c r="KT2" s="0"/>
+      <c r="KU2" s="0"/>
+      <c r="KV2" s="0"/>
+      <c r="KW2" s="0"/>
+      <c r="KX2" s="0"/>
+      <c r="KY2" s="0"/>
+      <c r="KZ2" s="0"/>
+      <c r="LA2" s="0"/>
+      <c r="LB2" s="0"/>
+      <c r="LC2" s="0"/>
+      <c r="LD2" s="0"/>
+      <c r="LE2" s="0"/>
+      <c r="LF2" s="0"/>
+      <c r="LG2" s="0"/>
+      <c r="LH2" s="0"/>
+      <c r="LI2" s="0"/>
+      <c r="LJ2" s="0"/>
+      <c r="LK2" s="0"/>
+      <c r="LL2" s="0"/>
+      <c r="LM2" s="0"/>
+      <c r="LN2" s="0"/>
+      <c r="LO2" s="0"/>
+      <c r="LP2" s="0"/>
+      <c r="LQ2" s="0"/>
+      <c r="LR2" s="0"/>
+      <c r="LS2" s="0"/>
+      <c r="LT2" s="0"/>
+      <c r="LU2" s="0"/>
+      <c r="LV2" s="0"/>
+      <c r="LW2" s="0"/>
+      <c r="LX2" s="0"/>
+      <c r="LY2" s="0"/>
+      <c r="LZ2" s="0"/>
+      <c r="MA2" s="0"/>
+      <c r="MB2" s="0"/>
+      <c r="MC2" s="0"/>
+      <c r="MD2" s="0"/>
+      <c r="ME2" s="0"/>
+      <c r="MF2" s="0"/>
+      <c r="MG2" s="0"/>
+      <c r="MH2" s="0"/>
+      <c r="MI2" s="0"/>
+      <c r="MJ2" s="0"/>
+      <c r="MK2" s="0"/>
+      <c r="ML2" s="0"/>
+      <c r="MM2" s="0"/>
+      <c r="MN2" s="0"/>
+      <c r="MO2" s="0"/>
+      <c r="MP2" s="0"/>
+      <c r="MQ2" s="0"/>
+      <c r="MR2" s="0"/>
+      <c r="MS2" s="0"/>
+      <c r="MT2" s="0"/>
+      <c r="MU2" s="0"/>
+      <c r="MV2" s="0"/>
+      <c r="MW2" s="0"/>
+      <c r="MX2" s="0"/>
+      <c r="MY2" s="0"/>
+      <c r="MZ2" s="0"/>
+      <c r="NA2" s="0"/>
+      <c r="NB2" s="0"/>
+      <c r="NC2" s="0"/>
+      <c r="ND2" s="0"/>
+      <c r="NE2" s="0"/>
+      <c r="NF2" s="0"/>
+      <c r="NG2" s="0"/>
+      <c r="NH2" s="0"/>
+      <c r="NI2" s="0"/>
+      <c r="NJ2" s="0"/>
+      <c r="NK2" s="0"/>
+      <c r="NL2" s="0"/>
+      <c r="NM2" s="0"/>
+      <c r="NN2" s="0"/>
+      <c r="NO2" s="0"/>
+      <c r="NP2" s="0"/>
+      <c r="NQ2" s="0"/>
+      <c r="NR2" s="0"/>
+      <c r="NS2" s="0"/>
+      <c r="NT2" s="0"/>
+      <c r="NU2" s="0"/>
+      <c r="NV2" s="0"/>
+      <c r="NW2" s="0"/>
+      <c r="NX2" s="0"/>
+      <c r="NY2" s="0"/>
+      <c r="NZ2" s="0"/>
+      <c r="OA2" s="0"/>
+      <c r="OB2" s="0"/>
+      <c r="OC2" s="0"/>
+      <c r="OD2" s="0"/>
+      <c r="OE2" s="0"/>
+      <c r="OF2" s="0"/>
+      <c r="OG2" s="0"/>
+      <c r="OH2" s="0"/>
+      <c r="OI2" s="0"/>
+      <c r="OJ2" s="0"/>
+      <c r="OK2" s="0"/>
+      <c r="OL2" s="0"/>
+      <c r="OM2" s="0"/>
+      <c r="ON2" s="0"/>
+      <c r="OO2" s="0"/>
+      <c r="OP2" s="0"/>
+      <c r="OQ2" s="0"/>
+      <c r="OR2" s="0"/>
+      <c r="OS2" s="0"/>
+      <c r="OT2" s="0"/>
+      <c r="OU2" s="0"/>
+      <c r="OV2" s="0"/>
+      <c r="OW2" s="0"/>
+      <c r="OX2" s="0"/>
+      <c r="OY2" s="0"/>
+      <c r="OZ2" s="0"/>
+      <c r="PA2" s="0"/>
+      <c r="PB2" s="0"/>
+      <c r="PC2" s="0"/>
+      <c r="PD2" s="0"/>
+      <c r="PE2" s="0"/>
+      <c r="PF2" s="0"/>
+      <c r="PG2" s="0"/>
+      <c r="PH2" s="0"/>
+      <c r="PI2" s="0"/>
+      <c r="PJ2" s="0"/>
+      <c r="PK2" s="0"/>
+      <c r="PL2" s="0"/>
+      <c r="PM2" s="0"/>
+      <c r="PN2" s="0"/>
+      <c r="PO2" s="0"/>
+      <c r="PP2" s="0"/>
+      <c r="PQ2" s="0"/>
+      <c r="PR2" s="0"/>
+      <c r="PS2" s="0"/>
+      <c r="PT2" s="0"/>
+      <c r="PU2" s="0"/>
+      <c r="PV2" s="0"/>
+      <c r="PW2" s="0"/>
+      <c r="PX2" s="0"/>
+      <c r="PY2" s="0"/>
+      <c r="PZ2" s="0"/>
+      <c r="QA2" s="0"/>
+      <c r="QB2" s="0"/>
+      <c r="QC2" s="0"/>
+      <c r="QD2" s="0"/>
+      <c r="QE2" s="0"/>
+      <c r="QF2" s="0"/>
+      <c r="QG2" s="0"/>
+      <c r="QH2" s="0"/>
+      <c r="QI2" s="0"/>
+      <c r="QJ2" s="0"/>
+      <c r="QK2" s="0"/>
+      <c r="QL2" s="0"/>
+      <c r="QM2" s="0"/>
+      <c r="QN2" s="0"/>
+      <c r="QO2" s="0"/>
+      <c r="QP2" s="0"/>
+      <c r="QQ2" s="0"/>
+      <c r="QR2" s="0"/>
+      <c r="QS2" s="0"/>
+      <c r="QT2" s="0"/>
+      <c r="QU2" s="0"/>
+      <c r="QV2" s="0"/>
+      <c r="QW2" s="0"/>
+      <c r="QX2" s="0"/>
+      <c r="QY2" s="0"/>
+      <c r="QZ2" s="0"/>
+      <c r="RA2" s="0"/>
+      <c r="RB2" s="0"/>
+      <c r="RC2" s="0"/>
+      <c r="RD2" s="0"/>
+      <c r="RE2" s="0"/>
+      <c r="RF2" s="0"/>
+      <c r="RG2" s="0"/>
+      <c r="RH2" s="0"/>
+      <c r="RI2" s="0"/>
+      <c r="RJ2" s="0"/>
+      <c r="RK2" s="0"/>
+      <c r="RL2" s="0"/>
+      <c r="RM2" s="0"/>
+      <c r="RN2" s="0"/>
+      <c r="RO2" s="0"/>
+      <c r="RP2" s="0"/>
+      <c r="RQ2" s="0"/>
+      <c r="RR2" s="0"/>
+      <c r="RS2" s="0"/>
+      <c r="RT2" s="0"/>
+      <c r="RU2" s="0"/>
+      <c r="RV2" s="0"/>
+      <c r="RW2" s="0"/>
+      <c r="RX2" s="0"/>
+      <c r="RY2" s="0"/>
+      <c r="RZ2" s="0"/>
+      <c r="SA2" s="0"/>
+      <c r="SB2" s="0"/>
+      <c r="SC2" s="0"/>
+      <c r="SD2" s="0"/>
+      <c r="SE2" s="0"/>
+      <c r="SF2" s="0"/>
+      <c r="SG2" s="0"/>
+      <c r="SH2" s="0"/>
+      <c r="SI2" s="0"/>
+      <c r="SJ2" s="0"/>
+      <c r="SK2" s="0"/>
+      <c r="SL2" s="0"/>
+      <c r="SM2" s="0"/>
+      <c r="SN2" s="0"/>
+      <c r="SO2" s="0"/>
+      <c r="SP2" s="0"/>
+      <c r="SQ2" s="0"/>
+      <c r="SR2" s="0"/>
+      <c r="SS2" s="0"/>
+      <c r="ST2" s="0"/>
+      <c r="SU2" s="0"/>
+      <c r="SV2" s="0"/>
+      <c r="SW2" s="0"/>
+      <c r="SX2" s="0"/>
+      <c r="SY2" s="0"/>
+      <c r="SZ2" s="0"/>
+      <c r="TA2" s="0"/>
+      <c r="TB2" s="0"/>
+      <c r="TC2" s="0"/>
+      <c r="TD2" s="0"/>
+      <c r="TE2" s="0"/>
+      <c r="TF2" s="0"/>
+      <c r="TG2" s="0"/>
+      <c r="TH2" s="0"/>
+      <c r="TI2" s="0"/>
+      <c r="TJ2" s="0"/>
+      <c r="TK2" s="0"/>
+      <c r="TL2" s="0"/>
+      <c r="TM2" s="0"/>
+      <c r="TN2" s="0"/>
+      <c r="TO2" s="0"/>
+      <c r="TP2" s="0"/>
+      <c r="TQ2" s="0"/>
+      <c r="TR2" s="0"/>
+      <c r="TS2" s="0"/>
+      <c r="TT2" s="0"/>
+      <c r="TU2" s="0"/>
+      <c r="TV2" s="0"/>
+      <c r="TW2" s="0"/>
+      <c r="TX2" s="0"/>
+      <c r="TY2" s="0"/>
+      <c r="TZ2" s="0"/>
+      <c r="UA2" s="0"/>
+      <c r="UB2" s="0"/>
+      <c r="UC2" s="0"/>
+      <c r="UD2" s="0"/>
+      <c r="UE2" s="0"/>
+      <c r="UF2" s="0"/>
+      <c r="UG2" s="0"/>
+      <c r="UH2" s="0"/>
+      <c r="UI2" s="0"/>
+      <c r="UJ2" s="0"/>
+      <c r="UK2" s="0"/>
+      <c r="UL2" s="0"/>
+      <c r="UM2" s="0"/>
+      <c r="UN2" s="0"/>
+      <c r="UO2" s="0"/>
+      <c r="UP2" s="0"/>
+      <c r="UQ2" s="0"/>
+      <c r="UR2" s="0"/>
+      <c r="US2" s="0"/>
+      <c r="UT2" s="0"/>
+      <c r="UU2" s="0"/>
+      <c r="UV2" s="0"/>
+      <c r="UW2" s="0"/>
+      <c r="UX2" s="0"/>
+      <c r="UY2" s="0"/>
+      <c r="UZ2" s="0"/>
+      <c r="VA2" s="0"/>
+      <c r="VB2" s="0"/>
+      <c r="VC2" s="0"/>
+      <c r="VD2" s="0"/>
+      <c r="VE2" s="0"/>
+      <c r="VF2" s="0"/>
+      <c r="VG2" s="0"/>
+      <c r="VH2" s="0"/>
+      <c r="VI2" s="0"/>
+      <c r="VJ2" s="0"/>
+      <c r="VK2" s="0"/>
+      <c r="VL2" s="0"/>
+      <c r="VM2" s="0"/>
+      <c r="VN2" s="0"/>
+      <c r="VO2" s="0"/>
+      <c r="VP2" s="0"/>
+      <c r="VQ2" s="0"/>
+      <c r="VR2" s="0"/>
+      <c r="VS2" s="0"/>
+      <c r="VT2" s="0"/>
+      <c r="VU2" s="0"/>
+      <c r="VV2" s="0"/>
+      <c r="VW2" s="0"/>
+      <c r="VX2" s="0"/>
+      <c r="VY2" s="0"/>
+      <c r="VZ2" s="0"/>
+      <c r="WA2" s="0"/>
+      <c r="WB2" s="0"/>
+      <c r="WC2" s="0"/>
+      <c r="WD2" s="0"/>
+      <c r="WE2" s="0"/>
+      <c r="WF2" s="0"/>
+      <c r="WG2" s="0"/>
+      <c r="WH2" s="0"/>
+      <c r="WI2" s="0"/>
+      <c r="WJ2" s="0"/>
+      <c r="WK2" s="0"/>
+      <c r="WL2" s="0"/>
+      <c r="WM2" s="0"/>
+      <c r="WN2" s="0"/>
+      <c r="WO2" s="0"/>
+      <c r="WP2" s="0"/>
+      <c r="WQ2" s="0"/>
+      <c r="WR2" s="0"/>
+      <c r="WS2" s="0"/>
+      <c r="WT2" s="0"/>
+      <c r="WU2" s="0"/>
+      <c r="WV2" s="0"/>
+      <c r="WW2" s="0"/>
+      <c r="WX2" s="0"/>
+      <c r="WY2" s="0"/>
+      <c r="WZ2" s="0"/>
+      <c r="XA2" s="0"/>
+      <c r="XB2" s="0"/>
+      <c r="XC2" s="0"/>
+      <c r="XD2" s="0"/>
+      <c r="XE2" s="0"/>
+      <c r="XF2" s="0"/>
+      <c r="XG2" s="0"/>
+      <c r="XH2" s="0"/>
+      <c r="XI2" s="0"/>
+      <c r="XJ2" s="0"/>
+      <c r="XK2" s="0"/>
+      <c r="XL2" s="0"/>
+      <c r="XM2" s="0"/>
+      <c r="XN2" s="0"/>
+      <c r="XO2" s="0"/>
+      <c r="XP2" s="0"/>
+      <c r="XQ2" s="0"/>
+      <c r="XR2" s="0"/>
+      <c r="XS2" s="0"/>
+      <c r="XT2" s="0"/>
+      <c r="XU2" s="0"/>
+      <c r="XV2" s="0"/>
+      <c r="XW2" s="0"/>
+      <c r="XX2" s="0"/>
+      <c r="XY2" s="0"/>
+      <c r="XZ2" s="0"/>
+      <c r="YA2" s="0"/>
+      <c r="YB2" s="0"/>
+      <c r="YC2" s="0"/>
+      <c r="YD2" s="0"/>
+      <c r="YE2" s="0"/>
+      <c r="YF2" s="0"/>
+      <c r="YG2" s="0"/>
+      <c r="YH2" s="0"/>
+      <c r="YI2" s="0"/>
+      <c r="YJ2" s="0"/>
+      <c r="YK2" s="0"/>
+      <c r="YL2" s="0"/>
+      <c r="YM2" s="0"/>
+      <c r="YN2" s="0"/>
+      <c r="YO2" s="0"/>
+      <c r="YP2" s="0"/>
+      <c r="YQ2" s="0"/>
+      <c r="YR2" s="0"/>
+      <c r="YS2" s="0"/>
+      <c r="YT2" s="0"/>
+      <c r="YU2" s="0"/>
+      <c r="YV2" s="0"/>
+      <c r="YW2" s="0"/>
+      <c r="YX2" s="0"/>
+      <c r="YY2" s="0"/>
+      <c r="YZ2" s="0"/>
+      <c r="ZA2" s="0"/>
+      <c r="ZB2" s="0"/>
+      <c r="ZC2" s="0"/>
+      <c r="ZD2" s="0"/>
+      <c r="ZE2" s="0"/>
+      <c r="ZF2" s="0"/>
+      <c r="ZG2" s="0"/>
+      <c r="ZH2" s="0"/>
+      <c r="ZI2" s="0"/>
+      <c r="ZJ2" s="0"/>
+      <c r="ZK2" s="0"/>
+      <c r="ZL2" s="0"/>
+      <c r="ZM2" s="0"/>
+      <c r="ZN2" s="0"/>
+      <c r="ZO2" s="0"/>
+      <c r="ZP2" s="0"/>
+      <c r="ZQ2" s="0"/>
+      <c r="ZR2" s="0"/>
+      <c r="ZS2" s="0"/>
+      <c r="ZT2" s="0"/>
+      <c r="ZU2" s="0"/>
+      <c r="ZV2" s="0"/>
+      <c r="ZW2" s="0"/>
+      <c r="ZX2" s="0"/>
+      <c r="ZY2" s="0"/>
+      <c r="ZZ2" s="0"/>
+      <c r="AAA2" s="0"/>
+      <c r="AAB2" s="0"/>
+      <c r="AAC2" s="0"/>
+      <c r="AAD2" s="0"/>
+      <c r="AAE2" s="0"/>
+      <c r="AAF2" s="0"/>
+      <c r="AAG2" s="0"/>
+      <c r="AAH2" s="0"/>
+      <c r="AAI2" s="0"/>
+      <c r="AAJ2" s="0"/>
+      <c r="AAK2" s="0"/>
+      <c r="AAL2" s="0"/>
+      <c r="AAM2" s="0"/>
+      <c r="AAN2" s="0"/>
+      <c r="AAO2" s="0"/>
+      <c r="AAP2" s="0"/>
+      <c r="AAQ2" s="0"/>
+      <c r="AAR2" s="0"/>
+      <c r="AAS2" s="0"/>
+      <c r="AAT2" s="0"/>
+      <c r="AAU2" s="0"/>
+      <c r="AAV2" s="0"/>
+      <c r="AAW2" s="0"/>
+      <c r="AAX2" s="0"/>
+      <c r="AAY2" s="0"/>
+      <c r="AAZ2" s="0"/>
+      <c r="ABA2" s="0"/>
+      <c r="ABB2" s="0"/>
+      <c r="ABC2" s="0"/>
+      <c r="ABD2" s="0"/>
+      <c r="ABE2" s="0"/>
+      <c r="ABF2" s="0"/>
+      <c r="ABG2" s="0"/>
+      <c r="ABH2" s="0"/>
+      <c r="ABI2" s="0"/>
+      <c r="ABJ2" s="0"/>
+      <c r="ABK2" s="0"/>
+      <c r="ABL2" s="0"/>
+      <c r="ABM2" s="0"/>
+      <c r="ABN2" s="0"/>
+      <c r="ABO2" s="0"/>
+      <c r="ABP2" s="0"/>
+      <c r="ABQ2" s="0"/>
+      <c r="ABR2" s="0"/>
+      <c r="ABS2" s="0"/>
+      <c r="ABT2" s="0"/>
+      <c r="ABU2" s="0"/>
+      <c r="ABV2" s="0"/>
+      <c r="ABW2" s="0"/>
+      <c r="ABX2" s="0"/>
+      <c r="ABY2" s="0"/>
+      <c r="ABZ2" s="0"/>
+      <c r="ACA2" s="0"/>
+      <c r="ACB2" s="0"/>
+      <c r="ACC2" s="0"/>
+      <c r="ACD2" s="0"/>
+      <c r="ACE2" s="0"/>
+      <c r="ACF2" s="0"/>
+      <c r="ACG2" s="0"/>
+      <c r="ACH2" s="0"/>
+      <c r="ACI2" s="0"/>
+      <c r="ACJ2" s="0"/>
+      <c r="ACK2" s="0"/>
+      <c r="ACL2" s="0"/>
+      <c r="ACM2" s="0"/>
+      <c r="ACN2" s="0"/>
+      <c r="ACO2" s="0"/>
+      <c r="ACP2" s="0"/>
+      <c r="ACQ2" s="0"/>
+      <c r="ACR2" s="0"/>
+      <c r="ACS2" s="0"/>
+      <c r="ACT2" s="0"/>
+      <c r="ACU2" s="0"/>
+      <c r="ACV2" s="0"/>
+      <c r="ACW2" s="0"/>
+      <c r="ACX2" s="0"/>
+      <c r="ACY2" s="0"/>
+      <c r="ACZ2" s="0"/>
+      <c r="ADA2" s="0"/>
+      <c r="ADB2" s="0"/>
+      <c r="ADC2" s="0"/>
+      <c r="ADD2" s="0"/>
+      <c r="ADE2" s="0"/>
+      <c r="ADF2" s="0"/>
+      <c r="ADG2" s="0"/>
+      <c r="ADH2" s="0"/>
+      <c r="ADI2" s="0"/>
+      <c r="ADJ2" s="0"/>
+      <c r="ADK2" s="0"/>
+      <c r="ADL2" s="0"/>
+      <c r="ADM2" s="0"/>
+      <c r="ADN2" s="0"/>
+      <c r="ADO2" s="0"/>
+      <c r="ADP2" s="0"/>
+      <c r="ADQ2" s="0"/>
+      <c r="ADR2" s="0"/>
+      <c r="ADS2" s="0"/>
+      <c r="ADT2" s="0"/>
+      <c r="ADU2" s="0"/>
+      <c r="ADV2" s="0"/>
+      <c r="ADW2" s="0"/>
+      <c r="ADX2" s="0"/>
+      <c r="ADY2" s="0"/>
+      <c r="ADZ2" s="0"/>
+      <c r="AEA2" s="0"/>
+      <c r="AEB2" s="0"/>
+      <c r="AEC2" s="0"/>
+      <c r="AED2" s="0"/>
+      <c r="AEE2" s="0"/>
+      <c r="AEF2" s="0"/>
+      <c r="AEG2" s="0"/>
+      <c r="AEH2" s="0"/>
+      <c r="AEI2" s="0"/>
+      <c r="AEJ2" s="0"/>
+      <c r="AEK2" s="0"/>
+      <c r="AEL2" s="0"/>
+      <c r="AEM2" s="0"/>
+      <c r="AEN2" s="0"/>
+      <c r="AEO2" s="0"/>
+      <c r="AEP2" s="0"/>
+      <c r="AEQ2" s="0"/>
+      <c r="AER2" s="0"/>
+      <c r="AES2" s="0"/>
+      <c r="AET2" s="0"/>
+      <c r="AEU2" s="0"/>
+      <c r="AEV2" s="0"/>
+      <c r="AEW2" s="0"/>
+      <c r="AEX2" s="0"/>
+      <c r="AEY2" s="0"/>
+      <c r="AEZ2" s="0"/>
+      <c r="AFA2" s="0"/>
+      <c r="AFB2" s="0"/>
+      <c r="AFC2" s="0"/>
+      <c r="AFD2" s="0"/>
+      <c r="AFE2" s="0"/>
+      <c r="AFF2" s="0"/>
+      <c r="AFG2" s="0"/>
+      <c r="AFH2" s="0"/>
+      <c r="AFI2" s="0"/>
+      <c r="AFJ2" s="0"/>
+      <c r="AFK2" s="0"/>
+      <c r="AFL2" s="0"/>
+      <c r="AFM2" s="0"/>
+      <c r="AFN2" s="0"/>
+      <c r="AFO2" s="0"/>
+      <c r="AFP2" s="0"/>
+      <c r="AFQ2" s="0"/>
+      <c r="AFR2" s="0"/>
+      <c r="AFS2" s="0"/>
+      <c r="AFT2" s="0"/>
+      <c r="AFU2" s="0"/>
+      <c r="AFV2" s="0"/>
+      <c r="AFW2" s="0"/>
+      <c r="AFX2" s="0"/>
+      <c r="AFY2" s="0"/>
+      <c r="AFZ2" s="0"/>
+      <c r="AGA2" s="0"/>
+      <c r="AGB2" s="0"/>
+      <c r="AGC2" s="0"/>
+      <c r="AGD2" s="0"/>
+      <c r="AGE2" s="0"/>
+      <c r="AGF2" s="0"/>
+      <c r="AGG2" s="0"/>
+      <c r="AGH2" s="0"/>
+      <c r="AGI2" s="0"/>
+      <c r="AGJ2" s="0"/>
+      <c r="AGK2" s="0"/>
+      <c r="AGL2" s="0"/>
+      <c r="AGM2" s="0"/>
+      <c r="AGN2" s="0"/>
+      <c r="AGO2" s="0"/>
+      <c r="AGP2" s="0"/>
+      <c r="AGQ2" s="0"/>
+      <c r="AGR2" s="0"/>
+      <c r="AGS2" s="0"/>
+      <c r="AGT2" s="0"/>
+      <c r="AGU2" s="0"/>
+      <c r="AGV2" s="0"/>
+      <c r="AGW2" s="0"/>
+      <c r="AGX2" s="0"/>
+      <c r="AGY2" s="0"/>
+      <c r="AGZ2" s="0"/>
+      <c r="AHA2" s="0"/>
+      <c r="AHB2" s="0"/>
+      <c r="AHC2" s="0"/>
+      <c r="AHD2" s="0"/>
+      <c r="AHE2" s="0"/>
+      <c r="AHF2" s="0"/>
+      <c r="AHG2" s="0"/>
+      <c r="AHH2" s="0"/>
+      <c r="AHI2" s="0"/>
+      <c r="AHJ2" s="0"/>
+      <c r="AHK2" s="0"/>
+      <c r="AHL2" s="0"/>
+      <c r="AHM2" s="0"/>
+      <c r="AHN2" s="0"/>
+      <c r="AHO2" s="0"/>
+      <c r="AHP2" s="0"/>
+      <c r="AHQ2" s="0"/>
+      <c r="AHR2" s="0"/>
+      <c r="AHS2" s="0"/>
+      <c r="AHT2" s="0"/>
+      <c r="AHU2" s="0"/>
+      <c r="AHV2" s="0"/>
+      <c r="AHW2" s="0"/>
+      <c r="AHX2" s="0"/>
+      <c r="AHY2" s="0"/>
+      <c r="AHZ2" s="0"/>
+      <c r="AIA2" s="0"/>
+      <c r="AIB2" s="0"/>
+      <c r="AIC2" s="0"/>
+      <c r="AID2" s="0"/>
+      <c r="AIE2" s="0"/>
+      <c r="AIF2" s="0"/>
+      <c r="AIG2" s="0"/>
+      <c r="AIH2" s="0"/>
+      <c r="AII2" s="0"/>
+      <c r="AIJ2" s="0"/>
+      <c r="AIK2" s="0"/>
+      <c r="AIL2" s="0"/>
+      <c r="AIM2" s="0"/>
+      <c r="AIN2" s="0"/>
+      <c r="AIO2" s="0"/>
+      <c r="AIP2" s="0"/>
+      <c r="AIQ2" s="0"/>
+      <c r="AIR2" s="0"/>
+      <c r="AIS2" s="0"/>
+      <c r="AIT2" s="0"/>
+      <c r="AIU2" s="0"/>
+      <c r="AIV2" s="0"/>
+      <c r="AIW2" s="0"/>
+      <c r="AIX2" s="0"/>
+      <c r="AIY2" s="0"/>
+      <c r="AIZ2" s="0"/>
+      <c r="AJA2" s="0"/>
+      <c r="AJB2" s="0"/>
+      <c r="AJC2" s="0"/>
+      <c r="AJD2" s="0"/>
+      <c r="AJE2" s="0"/>
+      <c r="AJF2" s="0"/>
+      <c r="AJG2" s="0"/>
+      <c r="AJH2" s="0"/>
+      <c r="AJI2" s="0"/>
+      <c r="AJJ2" s="0"/>
+      <c r="AJK2" s="0"/>
+      <c r="AJL2" s="0"/>
+      <c r="AJM2" s="0"/>
+      <c r="AJN2" s="0"/>
+      <c r="AJO2" s="0"/>
+      <c r="AJP2" s="0"/>
+      <c r="AJQ2" s="0"/>
+      <c r="AJR2" s="0"/>
+      <c r="AJS2" s="0"/>
+      <c r="AJT2" s="0"/>
+      <c r="AJU2" s="0"/>
+      <c r="AJV2" s="0"/>
+      <c r="AJW2" s="0"/>
+      <c r="AJX2" s="0"/>
+      <c r="AJY2" s="0"/>
+      <c r="AJZ2" s="0"/>
+      <c r="AKA2" s="0"/>
+      <c r="AKB2" s="0"/>
+      <c r="AKC2" s="0"/>
+      <c r="AKD2" s="0"/>
+      <c r="AKE2" s="0"/>
+      <c r="AKF2" s="0"/>
+      <c r="AKG2" s="0"/>
+      <c r="AKH2" s="0"/>
+      <c r="AKI2" s="0"/>
+      <c r="AKJ2" s="0"/>
+      <c r="AKK2" s="0"/>
+      <c r="AKL2" s="0"/>
+      <c r="AKM2" s="0"/>
+      <c r="AKN2" s="0"/>
+      <c r="AKO2" s="0"/>
+      <c r="AKP2" s="0"/>
+      <c r="AKQ2" s="0"/>
+      <c r="AKR2" s="0"/>
+      <c r="AKS2" s="0"/>
+      <c r="AKT2" s="0"/>
+      <c r="AKU2" s="0"/>
+      <c r="AKV2" s="0"/>
+      <c r="AKW2" s="0"/>
+      <c r="AKX2" s="0"/>
+      <c r="AKY2" s="0"/>
+      <c r="AKZ2" s="0"/>
+      <c r="ALA2" s="0"/>
+      <c r="ALB2" s="0"/>
+      <c r="ALC2" s="0"/>
+      <c r="ALD2" s="0"/>
+      <c r="ALE2" s="0"/>
+      <c r="ALF2" s="0"/>
+      <c r="ALG2" s="0"/>
+      <c r="ALH2" s="0"/>
+      <c r="ALI2" s="0"/>
+      <c r="ALJ2" s="0"/>
+      <c r="ALK2" s="0"/>
+      <c r="ALL2" s="0"/>
+      <c r="ALM2" s="0"/>
+      <c r="ALN2" s="0"/>
+      <c r="ALO2" s="0"/>
+      <c r="ALP2" s="0"/>
+      <c r="ALQ2" s="0"/>
+      <c r="ALR2" s="0"/>
+      <c r="ALS2" s="0"/>
+      <c r="ALT2" s="0"/>
+      <c r="ALU2" s="0"/>
+      <c r="ALV2" s="0"/>
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C3" s="7" t="n">
         <v>0.44</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AMF2" s="0"/>
-      <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row r="3" s="4" customFormat="true" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="G3" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>3.24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="AMF3" s="0"/>
       <c r="AMG3" s="0"/>
@@ -1350,35 +2359,66 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="0"/>
+    <row r="4" s="5" customFormat="true" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="10" t="s">
-        <v>17</v>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5"/>
+      <c r="B6" s="11" t="s">
+        <v>18</v>
       </c>
-      <c r="C5" s="6" t="n">
-        <f aca="false">(C2*B2)+(C3*B3)</f>
+      <c r="C6" s="7" t="n">
+        <f aca="false">(C3*B3)+(C4*B4)</f>
         <v>6.92</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="0"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="0"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="http://portal.fciconnect.com/Comergent//fci/drawing/c-bmj-0082.pdf"/>
-    <hyperlink ref="G2" r:id="rId2" display="http://www.newark.com/fci/54601-906wplf/cat3-rj12-modular-jack-6-position/dp/51M7960?ost=54601-906WPLF&amp;selectedCategoryId=&amp;categoryName=All+Categories&amp;categoryNameResp=All+Categories"/>
-    <hyperlink ref="F3" r:id="rId3" display="http://www.farnell.com/cad/320900.pdf"/>
-    <hyperlink ref="G3" r:id="rId4" display="http://www.newark.com/samtec/fle-110-01-g-dv/board-board-connector-socket-20/dp/11P4413"/>
+    <hyperlink ref="F3" r:id="rId1" display="http://portal.fciconnect.com/Comergent//fci/drawing/c-bmj-0082.pdf"/>
+    <hyperlink ref="G3" r:id="rId2" display="http://www.newark.com/fci/54601-906wplf/cat3-rj12-modular-jack-6-position/dp/51M7960?ost=54601-906WPLF&amp;selectedCategoryId=&amp;categoryName=All+Categories&amp;categoryNameResp=All+Categories"/>
+    <hyperlink ref="F4" r:id="rId3" display="http://www.farnell.com/cad/320900.pdf"/>
+    <hyperlink ref="G4" r:id="rId4" display="http://www.newark.com/samtec/fle-110-01-g-dv/board-board-connector-socket-20/dp/11P4413"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>